<commit_message>
Contiuei a cena da dificuldade, mas ainda nao acabei
</commit_message>
<xml_diff>
--- a/curvas de bezier(bola).xlsx
+++ b/curvas de bezier(bola).xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\utilizador\Documents\GitHub\guardiao\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -77,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,12 +186,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -208,6 +197,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -271,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -323,7 +318,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -517,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -528,7 +523,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,78 +535,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>610</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>583</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>368</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>450</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>280</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>186</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="4">
         <v>429</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="4">
         <v>110</v>
       </c>
       <c r="I3" s="1">
@@ -619,28 +614,28 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="5">
         <v>610</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>583</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
         <v>485</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>444</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>390</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <v>216</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="4">
         <v>625</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="4">
         <v>110</v>
       </c>
       <c r="I4" s="1">
@@ -648,28 +643,28 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="5">
         <v>610</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>583</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>843</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>520</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="4">
         <v>975</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="4">
         <v>113</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="4">
         <v>800</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="4">
         <v>110</v>
       </c>
       <c r="I5" s="1">
@@ -677,28 +672,28 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>610</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="5">
         <v>583</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>474</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>520</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>355</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>340</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <v>429</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="4">
         <v>195</v>
       </c>
       <c r="I6" s="1">
@@ -706,28 +701,28 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>610</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>583</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>466</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>331</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <v>625</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="4">
         <v>195</v>
       </c>
       <c r="I7" s="1">
@@ -735,28 +730,28 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>610</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>583</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>830</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>547</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>954</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>306</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <v>800</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="4">
         <v>195</v>
       </c>
       <c r="I8" s="1">
@@ -764,28 +759,28 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>610</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>583</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>479</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>564</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>456</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>459</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <v>429</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="4">
         <v>290</v>
       </c>
       <c r="I9" s="1">
@@ -793,28 +788,28 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>610</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>583</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>700</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>476</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>690</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>352</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <v>625</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="4">
         <v>290</v>
       </c>
       <c r="I10" s="1">
@@ -822,26 +817,28 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>610</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>583</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="4">
         <v>893</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="4">
         <v>470</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="4">
         <v>969</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6">
+      <c r="F11" s="4">
+        <v>340</v>
+      </c>
+      <c r="G11" s="4">
         <v>800</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="4">
         <v>290</v>
       </c>
       <c r="I11" s="1">

</xml_diff>